<commit_message>
Updated xls, one proc, and one special insert sql.
</commit_message>
<xml_diff>
--- a/PulseBox/Documentation/PulseBox Bugs & Enhancement Requests - Master.xlsx
+++ b/PulseBox/Documentation/PulseBox Bugs & Enhancement Requests - Master.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DTM\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DTM\GitHub\dtmdropbox\PulseBox\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -13,9 +13,10 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$K$41</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$K$44</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="577" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="664" uniqueCount="202">
   <si>
     <t>Enhancement/Bug Description</t>
   </si>
@@ -104,9 +105,6 @@
     <t>Alex/Dave</t>
   </si>
   <si>
-    <t>Utilizing the powerpoint doc provided by Abdul impelement user input section for demo!   Dave has to create the proc(s) to insert data.</t>
-  </si>
-  <si>
     <t>When graph has single point it shows as empty!</t>
   </si>
   <si>
@@ -120,9 +118,6 @@
   </si>
   <si>
     <t>Alex/Naveen</t>
-  </si>
-  <si>
-    <t>Start researching and building PulseBox Mobile app immediately as it will make our demo much more powerful.</t>
   </si>
   <si>
     <t>Review, sign, and send back LLC information to LegalZoom</t>
@@ -234,9 +229,6 @@
   </si>
   <si>
     <t>Arch</t>
-  </si>
-  <si>
-    <t>Abdul/Dave</t>
   </si>
   <si>
     <t>As I was doing some heavy testing on 4/19 and with our new discussions on active notifications I realized it might be best to eliminate the attrition report all together.  Instead add question/question category report where user can choose which questions/categories to filter by.  The reasoning is users will have Active Notifications alert them if there is possible attrition issue and after that they can go to question/category report and figure out which questions they want to filter by.  This is an architeture issue and something dd and Axe need to discuss and come up with a suggestion.</t>
@@ -570,9 +562,6 @@
     <t xml:space="preserve">I ran attrition report as aebadi2 (emp_id 6029) and selected all departments and entire 2014 as date range and aggregate with all 5 charts select (avg,min,max.stddev,variance).  Problem is same exact chart shows for all of them.  Is this even possible?  After further discussion with team and testing realized graph is ok and proc is ok.  It's just that STDDEV and VARIANCE data are zero for these and graph not showing.  </t>
   </si>
   <si>
-    <t>Reseach &amp; build PulseBox Mobile App</t>
-  </si>
-  <si>
     <t>Handle bad data such as 15-25-2015 as date.  Related to "add default null", but this will be from web side.   Also, when leaving date fields empty it does not default to 45.  Default 45 is working now.  Only need to fix bad input data.  Not big deal so moving it to low priority and we'll deal with it later.</t>
   </si>
   <si>
@@ -586,6 +575,96 @@
   </si>
   <si>
     <t xml:space="preserve">Replace Attrition report with active notification and question/category report? </t>
+  </si>
+  <si>
+    <t>Utilizing the powerpoint doc provided by Abdul impelement user input section for demo!   Dave has to create the proc(s) to insert data.  6/1 date met with few major issues!</t>
+  </si>
+  <si>
+    <t>Single quote as input causes  error in: Provide Pulse, Enter Events, Send Questions</t>
+  </si>
+  <si>
+    <t>Alex/DD</t>
+  </si>
+  <si>
+    <t>Whenever you enter single quotes in the data (feedback, event name, event desc, question text) it errors.  For example, if you enter "This is who's it is", the "who's" causes it to error (single quotes after o).</t>
+  </si>
+  <si>
+    <t>Location Comparison can't hanlde more than one location</t>
+  </si>
+  <si>
+    <t>GUI</t>
+  </si>
+  <si>
+    <t>Need to test out multiple locations.  It was working before, but failed one time.</t>
+  </si>
+  <si>
+    <t>Forecast Report - make sense of it</t>
+  </si>
+  <si>
+    <t>Abdul/DD</t>
+  </si>
+  <si>
+    <t>Report displays nice graph, but need to understand the input and what graph represents.</t>
+  </si>
+  <si>
+    <t>Figure out Email issue</t>
+  </si>
+  <si>
+    <t>DB</t>
+  </si>
+  <si>
+    <t>Currently, cannot email out of the DTM database, so need to figure out a workaround.  May have to download stunnel from stunnel.org.  See link: http://monkeyonoracle.blogspot.com/2009/11/plsql-and-gmail-or-utlsmtp-with-ssl.html</t>
+  </si>
+  <si>
+    <t>Notification Report - Minor Issue</t>
+  </si>
+  <si>
+    <t>Notification report displays way more departments than user should see.  I logged in as aebadi (emp_id=6005, company_id=3002) and should only see one dept (Executive), but a bunch of departments showed up!</t>
+  </si>
+  <si>
+    <t>Proc</t>
+  </si>
+  <si>
+    <t>sp_InsertNotifications - additional code needed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DD… please add the code for avg participation.  Similar to what you have for avg pulse (&gt;2 and &lt;8).  </t>
+  </si>
+  <si>
+    <t>PulseBox Mobile - Research and build</t>
+  </si>
+  <si>
+    <t>Start Selling PulseBox!</t>
+  </si>
+  <si>
+    <t>Sale</t>
+  </si>
+  <si>
+    <t>Abdul/All</t>
+  </si>
+  <si>
+    <t>Now that we have met the all important 6/1 deadline, need to start selling it!  Will start with Sloane and then on to others.  :)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Add appropriate data to help get funcationality of PulseBox to potential  customers!  </t>
+  </si>
+  <si>
+    <t>Add more data for PulseBox</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Start researching and building PulseBox Mobile app immediately as it will make our demo much more powerful.  Look at Webview for simple one screen android app (this just copies our dtmdata.com to mobile).  </t>
+  </si>
+  <si>
+    <t>Display Custom Questions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Display the custom questions to appropriate employee when they login.  Somehow, make them aware that they have some unanswered questions and after they answer the questions remove that from them.  Only display these questions for the date range specified when the questions were created!  </t>
+  </si>
+  <si>
+    <t>Naveen continue to learn from Alex</t>
+  </si>
+  <si>
+    <t>Continue to learn from Alex, so you can start making changes to the UI and we are not always having to go to Alex.</t>
   </si>
 </sst>
 </file>
@@ -676,7 +755,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -697,6 +776,18 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="12" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="12" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="12" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="12" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -979,7 +1070,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K67"/>
+  <dimension ref="A1:K77"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -1037,105 +1128,105 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" s="2" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" s="2" customFormat="1" ht="36" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>23</v>
+        <v>173</v>
       </c>
       <c r="B2" s="3">
-        <v>42073</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>29</v>
+        <v>42156</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>20</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>21</v>
+        <v>35</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>16</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>24</v>
+        <v>174</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" s="2" customFormat="1" ht="60" x14ac:dyDescent="0.2">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" s="2" customFormat="1" ht="24" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>39</v>
+        <v>176</v>
       </c>
       <c r="B3" s="3">
-        <v>42094</v>
+        <v>42156</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>21</v>
+        <v>177</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>16</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" s="2" customFormat="1" ht="96" x14ac:dyDescent="0.2">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" s="2" customFormat="1" ht="24" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>36</v>
+        <v>179</v>
       </c>
       <c r="B4" s="3">
-        <v>42094</v>
+        <v>42156</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>20</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>37</v>
+        <v>177</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>16</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>13</v>
+        <v>180</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" s="2" customFormat="1" ht="84" x14ac:dyDescent="0.2">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" s="2" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>41</v>
+        <v>198</v>
       </c>
       <c r="B5" s="3">
-        <v>42092</v>
+        <v>42156</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>20</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>21</v>
@@ -1147,27 +1238,27 @@
         <v>16</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" s="2" customFormat="1" ht="96" x14ac:dyDescent="0.2">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" s="2" customFormat="1" ht="36" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>175</v>
+        <v>182</v>
       </c>
       <c r="B6" s="3">
-        <v>42113</v>
+        <v>42156</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>66</v>
+        <v>183</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>16</v>
@@ -1176,27 +1267,27 @@
         <v>16</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>67</v>
+        <v>17</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" s="2" customFormat="1" ht="36" x14ac:dyDescent="0.2">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" s="2" customFormat="1" ht="24" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>63</v>
+        <v>188</v>
       </c>
       <c r="B7" s="3">
-        <v>42113</v>
+        <v>42156</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>20</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>37</v>
+        <v>187</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>16</v>
@@ -1205,256 +1296,256 @@
         <v>16</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>64</v>
+        <v>102</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" ht="48" x14ac:dyDescent="0.2">
-      <c r="A8" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="B8" s="5">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" s="2" customFormat="1" ht="36" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="B8" s="3">
+        <v>42156</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" s="2" customFormat="1" ht="36" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B9" s="3">
+        <v>42113</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="K9" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" s="2" customFormat="1" ht="36" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="B10" s="3">
+        <v>42076</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="K10" s="2" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="B11" s="3">
+        <v>42156</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="K11" s="2" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" s="2" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="B12" s="3">
+        <v>42125</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="K12" s="2" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" s="2" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="B13" s="3">
+        <v>42156</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="K13" s="2" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+      <c r="A14" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B14" s="5">
         <v>42093</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C14" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D8" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="E8" s="4" t="s">
+      <c r="D14" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E14" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="F8" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="G8" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="H8" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="K8" s="4" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" ht="24" x14ac:dyDescent="0.2">
-      <c r="A9" s="4" t="s">
-        <v>172</v>
-      </c>
-      <c r="B9" s="5">
-        <v>42102</v>
-      </c>
-      <c r="C9" s="5" t="s">
+      <c r="F14" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H14" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="K14" s="4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="24" x14ac:dyDescent="0.2">
+      <c r="A15" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B15" s="5">
+        <v>42095</v>
+      </c>
+      <c r="C15" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D9" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="G9" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="H9" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="K9" s="4" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" ht="24" x14ac:dyDescent="0.2">
-      <c r="A10" s="4" t="s">
+      <c r="D15" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H15" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="B10" s="5">
-        <v>42095</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="E10" s="4" t="s">
+      <c r="K15" s="4" t="s">
         <v>33</v>
-      </c>
-      <c r="F10" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="G10" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="H10" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="K10" s="4" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" ht="36" x14ac:dyDescent="0.2">
-      <c r="A11" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="B11" s="5">
-        <v>42074</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="F11" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="G11" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="H11" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="K11" s="4" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A12" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="B12" s="5">
-        <v>42075</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="F12" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="G12" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="H12" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="K12" s="4" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" ht="48" x14ac:dyDescent="0.2">
-      <c r="A13" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B13" s="5">
-        <v>42089</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="F13" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="G13" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="H13" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="K13" s="4" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" ht="36" x14ac:dyDescent="0.2">
-      <c r="A14" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="B14" s="5">
-        <v>42089</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="F14" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="G14" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="H14" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="K14" s="4" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" ht="36" x14ac:dyDescent="0.2">
-      <c r="A15" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="B15" s="5">
-        <v>42096</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="F15" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="G15" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="H15" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="K15" s="4" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="36" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="B16" s="5">
-        <v>42113</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>12</v>
+        <v>42074</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>20</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E16" s="4" t="s">
         <v>21</v>
@@ -1466,82 +1557,82 @@
         <v>16</v>
       </c>
       <c r="H16" s="4" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="K16" s="4" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" ht="60" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" ht="48" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
-        <v>57</v>
+        <v>19</v>
       </c>
       <c r="B17" s="5">
-        <v>42113</v>
+        <v>42089</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>12</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="E17" s="4" t="s">
         <v>21</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G17" s="4" t="s">
         <v>16</v>
       </c>
       <c r="H17" s="4" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="K17" s="4" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" ht="24" x14ac:dyDescent="0.2">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" ht="36" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
-        <v>59</v>
+        <v>45</v>
       </c>
       <c r="B18" s="5">
-        <v>42113</v>
+        <v>42089</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>12</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>27</v>
+        <v>46</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G18" s="4" t="s">
         <v>16</v>
       </c>
       <c r="H18" s="4" t="s">
-        <v>17</v>
+        <v>46</v>
       </c>
       <c r="K18" s="4" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" ht="24" x14ac:dyDescent="0.2">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" ht="36" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="B19" s="5">
-        <v>42064</v>
-      </c>
-      <c r="C19" s="5" t="s">
+        <v>42096</v>
+      </c>
+      <c r="C19" s="4" t="s">
         <v>12</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>13</v>
+        <v>46</v>
       </c>
       <c r="E19" s="4" t="s">
         <v>21</v>
@@ -1553,15 +1644,15 @@
         <v>16</v>
       </c>
       <c r="H19" s="4" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="K19" s="4" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
     </row>
     <row r="20" spans="1:11" ht="36" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="B20" s="5">
         <v>42113</v>
@@ -1570,36 +1661,36 @@
         <v>12</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E20" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G20" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H20" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="K20" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="F20" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="G20" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="H20" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="K20" s="4" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" ht="36" x14ac:dyDescent="0.2">
+    </row>
+    <row r="21" spans="1:11" ht="60" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
-        <v>26</v>
+        <v>55</v>
       </c>
       <c r="B21" s="5">
-        <v>42074</v>
-      </c>
-      <c r="C21" s="5" t="s">
+        <v>42113</v>
+      </c>
+      <c r="C21" s="4" t="s">
         <v>12</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E21" s="4" t="s">
         <v>21</v>
@@ -1611,15 +1702,15 @@
         <v>16</v>
       </c>
       <c r="H21" s="4" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="K21" s="4" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" ht="24" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="B22" s="5">
         <v>42113</v>
@@ -1628,10 +1719,10 @@
         <v>12</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>54</v>
+        <v>35</v>
       </c>
       <c r="F22" s="4" t="s">
         <v>16</v>
@@ -1640,27 +1731,27 @@
         <v>16</v>
       </c>
       <c r="H22" s="4" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="K22" s="4" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" ht="36" x14ac:dyDescent="0.2">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" ht="24" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
-        <v>73</v>
+        <v>41</v>
       </c>
       <c r="B23" s="5">
-        <v>42088</v>
-      </c>
-      <c r="C23" s="4" t="s">
+        <v>42064</v>
+      </c>
+      <c r="C23" s="5" t="s">
         <v>12</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>74</v>
+        <v>13</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>75</v>
+        <v>21</v>
       </c>
       <c r="F23" s="4" t="s">
         <v>15</v>
@@ -1669,85 +1760,85 @@
         <v>16</v>
       </c>
       <c r="H23" s="4" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="K23" s="4" t="s">
-        <v>76</v>
+        <v>42</v>
       </c>
     </row>
     <row r="24" spans="1:11" ht="36" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
-        <v>77</v>
+        <v>59</v>
       </c>
       <c r="B24" s="5">
-        <v>42088</v>
+        <v>42113</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>78</v>
+        <v>52</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G24" s="4" t="s">
         <v>16</v>
       </c>
       <c r="H24" s="4" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="K24" s="4" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" ht="24" x14ac:dyDescent="0.2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" ht="36" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="s">
-        <v>170</v>
+        <v>25</v>
       </c>
       <c r="B25" s="5">
-        <v>42076</v>
+        <v>42074</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="E25" s="4" t="s">
         <v>21</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G25" s="4" t="s">
         <v>16</v>
       </c>
       <c r="H25" s="4" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="K25" s="4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" ht="36" x14ac:dyDescent="0.2">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" ht="48" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
-        <v>80</v>
+        <v>51</v>
       </c>
       <c r="B26" s="5">
-        <v>42093</v>
+        <v>42113</v>
       </c>
       <c r="C26" s="4" t="s">
         <v>12</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>21</v>
+        <v>52</v>
       </c>
       <c r="F26" s="4" t="s">
         <v>16</v>
@@ -1756,164 +1847,146 @@
         <v>16</v>
       </c>
       <c r="H26" s="4" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="K26" s="4" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" ht="36" x14ac:dyDescent="0.2">
       <c r="A27" s="4" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="B27" s="5">
-        <v>42096</v>
+        <v>42088</v>
       </c>
       <c r="C27" s="4" t="s">
         <v>12</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>48</v>
+        <v>71</v>
       </c>
       <c r="E27" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="F27" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G27" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H27" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="K27" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" ht="36" x14ac:dyDescent="0.2">
+      <c r="A28" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="B28" s="5">
+        <v>42088</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E28" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="F28" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G28" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H28" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="K28" s="4" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" ht="36" x14ac:dyDescent="0.2">
+      <c r="A29" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="B29" s="5">
+        <v>42093</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E29" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="F27" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="G27" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="H27" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="K27" s="4" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" s="6" customFormat="1" ht="36" x14ac:dyDescent="0.2">
-      <c r="A28" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="B28" s="7">
-        <v>42073</v>
-      </c>
-      <c r="C28" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="D28" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="E28" s="6" t="s">
+      <c r="F29" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G29" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H29" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="K29" s="4" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A30" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="B30" s="5">
+        <v>42096</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="E30" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="F28" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="G28" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="H28" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="I28" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="J28" s="7">
-        <v>42087</v>
-      </c>
-      <c r="K28" s="6" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" s="6" customFormat="1" ht="24" x14ac:dyDescent="0.2">
-      <c r="A29" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="B29" s="7">
-        <v>42064</v>
-      </c>
-      <c r="C29" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="D29" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="E29" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="F29" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="G29" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="H29" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="I29" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="J29" s="7">
-        <v>42075</v>
-      </c>
-      <c r="K29" s="6" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" s="6" customFormat="1" ht="96" x14ac:dyDescent="0.2">
-      <c r="A30" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="B30" s="7">
-        <v>42073</v>
-      </c>
-      <c r="C30" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="D30" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="E30" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="F30" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="G30" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="H30" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="I30" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="J30" s="7">
-        <v>42075</v>
-      </c>
-      <c r="K30" s="6" t="s">
-        <v>91</v>
+      <c r="F30" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G30" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H30" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="K30" s="4" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="31" spans="1:11" s="6" customFormat="1" ht="36" x14ac:dyDescent="0.2">
       <c r="A31" s="6" t="s">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="B31" s="7">
         <v>42073</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D31" s="6" t="s">
-        <v>27</v>
+        <v>82</v>
       </c>
       <c r="E31" s="6" t="s">
         <v>21</v>
       </c>
       <c r="F31" s="6" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G31" s="6" t="s">
         <v>15</v>
@@ -1925,91 +1998,94 @@
         <v>22</v>
       </c>
       <c r="J31" s="7">
-        <v>42076</v>
+        <v>42087</v>
       </c>
       <c r="K31" s="6" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11" s="6" customFormat="1" ht="60" x14ac:dyDescent="0.2">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" s="6" customFormat="1" ht="24" x14ac:dyDescent="0.2">
       <c r="A32" s="6" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="B32" s="7">
-        <v>42073</v>
+        <v>42064</v>
       </c>
       <c r="C32" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D32" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E32" s="6" t="s">
         <v>21</v>
       </c>
       <c r="F32" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G32" s="6" t="s">
         <v>15</v>
       </c>
       <c r="H32" s="6" t="s">
-        <v>13</v>
+        <v>22</v>
+      </c>
+      <c r="I32" s="6" t="s">
+        <v>22</v>
       </c>
       <c r="J32" s="7">
-        <v>42088</v>
+        <v>42075</v>
       </c>
       <c r="K32" s="6" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="33" spans="1:11" s="6" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" s="6" customFormat="1" ht="96" x14ac:dyDescent="0.2">
       <c r="A33" s="6" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="B33" s="7">
-        <v>42064</v>
+        <v>42073</v>
       </c>
       <c r="C33" s="7" t="s">
         <v>20</v>
       </c>
       <c r="D33" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="E33" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="F33" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="G33" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="H33" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="I33" s="6" t="s">
         <v>13</v>
-      </c>
-      <c r="E33" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="F33" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="G33" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="H33" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="I33" s="6" t="s">
-        <v>22</v>
       </c>
       <c r="J33" s="7">
         <v>42075</v>
       </c>
       <c r="K33" s="6" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="34" spans="1:11" s="6" customFormat="1" ht="72" x14ac:dyDescent="0.2">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" s="6" customFormat="1" ht="36" x14ac:dyDescent="0.2">
       <c r="A34" s="6" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="B34" s="7">
         <v>42073</v>
       </c>
       <c r="C34" s="7" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="D34" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E34" s="6" t="s">
         <v>21</v>
@@ -2027,27 +2103,27 @@
         <v>22</v>
       </c>
       <c r="J34" s="7">
-        <v>42087</v>
+        <v>42076</v>
       </c>
       <c r="K34" s="6" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="35" spans="1:11" s="6" customFormat="1" ht="93.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" s="6" customFormat="1" ht="60" x14ac:dyDescent="0.2">
       <c r="A35" s="6" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="B35" s="7">
-        <v>42074</v>
+        <v>42073</v>
       </c>
       <c r="C35" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D35" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E35" s="6" t="s">
-        <v>49</v>
+        <v>21</v>
       </c>
       <c r="F35" s="6" t="s">
         <v>16</v>
@@ -2056,24 +2132,21 @@
         <v>15</v>
       </c>
       <c r="H35" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="I35" s="6" t="s">
-        <v>48</v>
+        <v>13</v>
       </c>
       <c r="J35" s="7">
-        <v>42087</v>
+        <v>42088</v>
       </c>
       <c r="K35" s="6" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
     </row>
     <row r="36" spans="1:11" s="6" customFormat="1" ht="24" x14ac:dyDescent="0.2">
       <c r="A36" s="6" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="B36" s="7">
-        <v>42075</v>
+        <v>42064</v>
       </c>
       <c r="C36" s="7" t="s">
         <v>20</v>
@@ -2100,27 +2173,27 @@
         <v>42075</v>
       </c>
       <c r="K36" s="6" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="37" spans="1:11" s="6" customFormat="1" ht="36" x14ac:dyDescent="0.2">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" s="6" customFormat="1" ht="72" x14ac:dyDescent="0.2">
       <c r="A37" s="6" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="B37" s="7">
-        <v>42080</v>
+        <v>42073</v>
       </c>
       <c r="C37" s="7" t="s">
         <v>20</v>
       </c>
       <c r="D37" s="6" t="s">
-        <v>105</v>
+        <v>26</v>
       </c>
       <c r="E37" s="6" t="s">
-        <v>75</v>
+        <v>21</v>
       </c>
       <c r="F37" s="6" t="s">
-        <v>106</v>
+        <v>15</v>
       </c>
       <c r="G37" s="6" t="s">
         <v>15</v>
@@ -2135,59 +2208,59 @@
         <v>42087</v>
       </c>
       <c r="K37" s="6" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="38" spans="1:11" s="6" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" s="6" customFormat="1" ht="93.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="6" t="s">
-        <v>108</v>
+        <v>97</v>
       </c>
       <c r="B38" s="7">
-        <v>42080</v>
+        <v>42074</v>
       </c>
       <c r="C38" s="7" t="s">
-        <v>12</v>
+        <v>28</v>
       </c>
       <c r="D38" s="6" t="s">
-        <v>105</v>
+        <v>26</v>
       </c>
       <c r="E38" s="6" t="s">
-        <v>75</v>
+        <v>47</v>
       </c>
       <c r="F38" s="6" t="s">
-        <v>106</v>
+        <v>16</v>
       </c>
       <c r="G38" s="6" t="s">
         <v>15</v>
       </c>
       <c r="H38" s="6" t="s">
-        <v>22</v>
+        <v>46</v>
       </c>
       <c r="I38" s="6" t="s">
-        <v>22</v>
+        <v>46</v>
       </c>
       <c r="J38" s="7">
-        <v>42089</v>
+        <v>42087</v>
       </c>
       <c r="K38" s="6" t="s">
-        <v>109</v>
+        <v>98</v>
       </c>
     </row>
     <row r="39" spans="1:11" s="6" customFormat="1" ht="24" x14ac:dyDescent="0.2">
       <c r="A39" s="6" t="s">
-        <v>110</v>
+        <v>99</v>
       </c>
       <c r="B39" s="7">
-        <v>42088</v>
-      </c>
-      <c r="C39" s="6" t="s">
+        <v>42075</v>
+      </c>
+      <c r="C39" s="7" t="s">
         <v>20</v>
       </c>
       <c r="D39" s="6" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="E39" s="6" t="s">
-        <v>75</v>
+        <v>21</v>
       </c>
       <c r="F39" s="6" t="s">
         <v>15</v>
@@ -2202,30 +2275,30 @@
         <v>22</v>
       </c>
       <c r="J39" s="7">
-        <v>42089</v>
+        <v>42075</v>
       </c>
       <c r="K39" s="6" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="40" spans="1:11" s="6" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" s="6" customFormat="1" ht="36" x14ac:dyDescent="0.2">
       <c r="A40" s="6" t="s">
-        <v>112</v>
+        <v>101</v>
       </c>
       <c r="B40" s="7">
-        <v>42088</v>
-      </c>
-      <c r="C40" s="6" t="s">
+        <v>42080</v>
+      </c>
+      <c r="C40" s="7" t="s">
         <v>20</v>
       </c>
       <c r="D40" s="6" t="s">
-        <v>27</v>
+        <v>102</v>
       </c>
       <c r="E40" s="6" t="s">
-        <v>21</v>
+        <v>72</v>
       </c>
       <c r="F40" s="6" t="s">
-        <v>16</v>
+        <v>103</v>
       </c>
       <c r="G40" s="6" t="s">
         <v>15</v>
@@ -2237,30 +2310,30 @@
         <v>22</v>
       </c>
       <c r="J40" s="7">
-        <v>42089</v>
+        <v>42087</v>
       </c>
       <c r="K40" s="6" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
     </row>
     <row r="41" spans="1:11" s="6" customFormat="1" ht="24" x14ac:dyDescent="0.2">
       <c r="A41" s="6" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="B41" s="7">
-        <v>42088</v>
-      </c>
-      <c r="C41" s="6" t="s">
-        <v>20</v>
+        <v>42080</v>
+      </c>
+      <c r="C41" s="7" t="s">
+        <v>12</v>
       </c>
       <c r="D41" s="6" t="s">
-        <v>22</v>
+        <v>102</v>
       </c>
       <c r="E41" s="6" t="s">
-        <v>21</v>
+        <v>72</v>
       </c>
       <c r="F41" s="6" t="s">
-        <v>15</v>
+        <v>103</v>
       </c>
       <c r="G41" s="6" t="s">
         <v>15</v>
@@ -2275,27 +2348,27 @@
         <v>42089</v>
       </c>
       <c r="K41" s="6" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
     </row>
     <row r="42" spans="1:11" s="6" customFormat="1" ht="24" x14ac:dyDescent="0.2">
       <c r="A42" s="6" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="B42" s="7">
-        <v>42073</v>
-      </c>
-      <c r="C42" s="7" t="s">
-        <v>29</v>
+        <v>42088</v>
+      </c>
+      <c r="C42" s="6" t="s">
+        <v>20</v>
       </c>
       <c r="D42" s="6" t="s">
-        <v>85</v>
+        <v>26</v>
       </c>
       <c r="E42" s="6" t="s">
-        <v>21</v>
+        <v>72</v>
       </c>
       <c r="F42" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G42" s="6" t="s">
         <v>15</v>
@@ -2307,24 +2380,24 @@
         <v>22</v>
       </c>
       <c r="J42" s="7">
-        <v>42091</v>
+        <v>42089</v>
       </c>
       <c r="K42" s="6" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="43" spans="1:11" s="6" customFormat="1" ht="36" x14ac:dyDescent="0.2">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" s="6" customFormat="1" ht="24" x14ac:dyDescent="0.2">
       <c r="A43" s="6" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="B43" s="7">
-        <v>42074</v>
-      </c>
-      <c r="C43" s="7" t="s">
-        <v>12</v>
+        <v>42088</v>
+      </c>
+      <c r="C43" s="6" t="s">
+        <v>20</v>
       </c>
       <c r="D43" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E43" s="6" t="s">
         <v>21</v>
@@ -2342,30 +2415,30 @@
         <v>22</v>
       </c>
       <c r="J43" s="7">
-        <v>42091</v>
+        <v>42089</v>
       </c>
       <c r="K43" s="6" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
     </row>
     <row r="44" spans="1:11" s="6" customFormat="1" ht="24" x14ac:dyDescent="0.2">
       <c r="A44" s="6" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
       <c r="B44" s="7">
-        <v>42074</v>
-      </c>
-      <c r="C44" s="7" t="s">
-        <v>12</v>
+        <v>42088</v>
+      </c>
+      <c r="C44" s="6" t="s">
+        <v>20</v>
       </c>
       <c r="D44" s="6" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="E44" s="6" t="s">
         <v>21</v>
       </c>
       <c r="F44" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G44" s="6" t="s">
         <v>15</v>
@@ -2377,30 +2450,30 @@
         <v>22</v>
       </c>
       <c r="J44" s="7">
-        <v>42091</v>
+        <v>42089</v>
       </c>
       <c r="K44" s="6" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="45" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.2">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" s="6" customFormat="1" ht="24" x14ac:dyDescent="0.2">
       <c r="A45" s="6" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
       <c r="B45" s="7">
-        <v>42088</v>
-      </c>
-      <c r="C45" s="6" t="s">
-        <v>20</v>
+        <v>42073</v>
+      </c>
+      <c r="C45" s="7" t="s">
+        <v>28</v>
       </c>
       <c r="D45" s="6" t="s">
-        <v>17</v>
+        <v>82</v>
       </c>
       <c r="E45" s="6" t="s">
-        <v>75</v>
+        <v>21</v>
       </c>
       <c r="F45" s="6" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G45" s="6" t="s">
         <v>15</v>
@@ -2415,27 +2488,27 @@
         <v>42091</v>
       </c>
       <c r="K45" s="6" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="46" spans="1:11" s="6" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" s="6" customFormat="1" ht="36" x14ac:dyDescent="0.2">
       <c r="A46" s="6" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="B46" s="7">
-        <v>42088</v>
-      </c>
-      <c r="C46" s="6" t="s">
+        <v>42074</v>
+      </c>
+      <c r="C46" s="7" t="s">
         <v>12</v>
       </c>
       <c r="D46" s="6" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="E46" s="6" t="s">
-        <v>49</v>
+        <v>21</v>
       </c>
       <c r="F46" s="6" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G46" s="6" t="s">
         <v>15</v>
@@ -2450,21 +2523,21 @@
         <v>42091</v>
       </c>
       <c r="K46" s="6" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
     </row>
     <row r="47" spans="1:11" s="6" customFormat="1" ht="24" x14ac:dyDescent="0.2">
       <c r="A47" s="6" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
       <c r="B47" s="7">
-        <v>42088</v>
-      </c>
-      <c r="C47" s="6" t="s">
-        <v>20</v>
+        <v>42074</v>
+      </c>
+      <c r="C47" s="7" t="s">
+        <v>12</v>
       </c>
       <c r="D47" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E47" s="6" t="s">
         <v>21</v>
@@ -2485,59 +2558,62 @@
         <v>42091</v>
       </c>
       <c r="K47" s="6" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="48" spans="1:11" s="6" customFormat="1" ht="48" x14ac:dyDescent="0.2">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A48" s="6" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
       <c r="B48" s="7">
-        <v>42073</v>
-      </c>
-      <c r="C48" s="7" t="s">
+        <v>42088</v>
+      </c>
+      <c r="C48" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D48" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E48" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="F48" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="G48" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="H48" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="I48" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="J48" s="7">
+        <v>42091</v>
+      </c>
+      <c r="K48" s="6" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" s="6" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+      <c r="A49" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="B49" s="7">
+        <v>42088</v>
+      </c>
+      <c r="C49" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D48" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="E48" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="F48" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="G48" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="H48" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="J48" s="7">
-        <v>42092</v>
-      </c>
-      <c r="K48" s="6" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="49" spans="1:11" s="6" customFormat="1" ht="84" x14ac:dyDescent="0.2">
-      <c r="A49" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="B49" s="7">
-        <v>42073</v>
-      </c>
-      <c r="C49" s="7" t="s">
-        <v>12</v>
-      </c>
       <c r="D49" s="6" t="s">
-        <v>85</v>
+        <v>22</v>
       </c>
       <c r="E49" s="6" t="s">
-        <v>21</v>
+        <v>47</v>
       </c>
       <c r="F49" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G49" s="6" t="s">
         <v>15</v>
@@ -2549,15 +2625,15 @@
         <v>22</v>
       </c>
       <c r="J49" s="7">
-        <v>42092</v>
+        <v>42091</v>
       </c>
       <c r="K49" s="6" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
     </row>
     <row r="50" spans="1:11" s="6" customFormat="1" ht="24" x14ac:dyDescent="0.2">
       <c r="A50" s="6" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
       <c r="B50" s="7">
         <v>42088</v>
@@ -2566,115 +2642,112 @@
         <v>20</v>
       </c>
       <c r="D50" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E50" s="6" t="s">
-        <v>49</v>
+        <v>21</v>
       </c>
       <c r="F50" s="6" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G50" s="6" t="s">
         <v>15</v>
       </c>
       <c r="H50" s="6" t="s">
-        <v>48</v>
+        <v>22</v>
       </c>
       <c r="I50" s="6" t="s">
-        <v>48</v>
+        <v>22</v>
       </c>
       <c r="J50" s="7">
+        <v>42091</v>
+      </c>
+      <c r="K50" s="6" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" s="6" customFormat="1" ht="48" x14ac:dyDescent="0.2">
+      <c r="A51" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="B51" s="7">
+        <v>42073</v>
+      </c>
+      <c r="C51" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D51" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="E51" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="F51" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="G51" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="H51" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="J51" s="7">
         <v>42092</v>
       </c>
-      <c r="K50" s="6" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="51" spans="1:11" s="6" customFormat="1" ht="120" x14ac:dyDescent="0.2">
-      <c r="A51" s="6" t="s">
-        <v>134</v>
-      </c>
-      <c r="B51" s="7">
-        <v>42088</v>
-      </c>
-      <c r="C51" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="D51" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="E51" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="F51" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="G51" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="H51" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="I51" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="J51" s="7">
-        <v>42093</v>
-      </c>
       <c r="K51" s="6" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="52" spans="1:11" s="6" customFormat="1" ht="36" x14ac:dyDescent="0.2">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" s="6" customFormat="1" ht="84" x14ac:dyDescent="0.2">
       <c r="A52" s="6" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
       <c r="B52" s="7">
-        <v>42088</v>
-      </c>
-      <c r="C52" s="6" t="s">
-        <v>20</v>
+        <v>42073</v>
+      </c>
+      <c r="C52" s="7" t="s">
+        <v>12</v>
       </c>
       <c r="D52" s="6" t="s">
-        <v>13</v>
+        <v>82</v>
       </c>
       <c r="E52" s="6" t="s">
-        <v>49</v>
+        <v>21</v>
       </c>
       <c r="F52" s="6" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G52" s="6" t="s">
         <v>15</v>
       </c>
       <c r="H52" s="6" t="s">
-        <v>48</v>
+        <v>22</v>
       </c>
       <c r="I52" s="6" t="s">
-        <v>48</v>
+        <v>22</v>
       </c>
       <c r="J52" s="7">
-        <v>42094</v>
+        <v>42092</v>
       </c>
       <c r="K52" s="6" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
     </row>
     <row r="53" spans="1:11" s="6" customFormat="1" ht="24" x14ac:dyDescent="0.2">
       <c r="A53" s="6" t="s">
-        <v>138</v>
+        <v>129</v>
       </c>
       <c r="B53" s="7">
         <v>42088</v>
       </c>
       <c r="C53" s="6" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="D53" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E53" s="6" t="s">
-        <v>139</v>
+        <v>47</v>
       </c>
       <c r="F53" s="6" t="s">
         <v>15</v>
@@ -2683,103 +2756,103 @@
         <v>15</v>
       </c>
       <c r="H53" s="6" t="s">
-        <v>27</v>
+        <v>46</v>
       </c>
       <c r="I53" s="6" t="s">
-        <v>27</v>
+        <v>46</v>
       </c>
       <c r="J53" s="7">
-        <v>42094</v>
+        <v>42092</v>
       </c>
       <c r="K53" s="6" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="54" spans="1:11" s="6" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" s="6" customFormat="1" ht="120" x14ac:dyDescent="0.2">
       <c r="A54" s="6" t="s">
-        <v>141</v>
+        <v>131</v>
       </c>
       <c r="B54" s="7">
-        <v>42064</v>
-      </c>
-      <c r="C54" s="7" t="s">
-        <v>12</v>
+        <v>42088</v>
+      </c>
+      <c r="C54" s="6" t="s">
+        <v>28</v>
       </c>
       <c r="D54" s="6" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="E54" s="6" t="s">
-        <v>21</v>
+        <v>35</v>
       </c>
       <c r="F54" s="6" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G54" s="6" t="s">
         <v>15</v>
       </c>
       <c r="H54" s="6" t="s">
-        <v>142</v>
+        <v>24</v>
       </c>
       <c r="I54" s="6" t="s">
-        <v>17</v>
+        <v>46</v>
       </c>
       <c r="J54" s="7">
-        <v>42094</v>
+        <v>42093</v>
       </c>
       <c r="K54" s="6" t="s">
-        <v>143</v>
+        <v>132</v>
       </c>
     </row>
     <row r="55" spans="1:11" s="6" customFormat="1" ht="36" x14ac:dyDescent="0.2">
       <c r="A55" s="6" t="s">
-        <v>144</v>
+        <v>133</v>
       </c>
       <c r="B55" s="7">
-        <v>41709</v>
-      </c>
-      <c r="C55" s="7" t="s">
-        <v>12</v>
+        <v>42088</v>
+      </c>
+      <c r="C55" s="6" t="s">
+        <v>20</v>
       </c>
       <c r="D55" s="6" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="E55" s="6" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="F55" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G55" s="6" t="s">
         <v>15</v>
       </c>
       <c r="H55" s="6" t="s">
-        <v>17</v>
+        <v>46</v>
       </c>
       <c r="I55" s="6" t="s">
-        <v>17</v>
+        <v>46</v>
       </c>
       <c r="J55" s="7">
         <v>42094</v>
       </c>
       <c r="K55" s="6" t="s">
-        <v>145</v>
+        <v>134</v>
       </c>
     </row>
     <row r="56" spans="1:11" s="6" customFormat="1" ht="24" x14ac:dyDescent="0.2">
       <c r="A56" s="6" t="s">
-        <v>146</v>
+        <v>135</v>
       </c>
       <c r="B56" s="7">
-        <v>42064</v>
-      </c>
-      <c r="C56" s="7" t="s">
-        <v>20</v>
+        <v>42088</v>
+      </c>
+      <c r="C56" s="6" t="s">
+        <v>28</v>
       </c>
       <c r="D56" s="6" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="E56" s="6" t="s">
-        <v>54</v>
+        <v>136</v>
       </c>
       <c r="F56" s="6" t="s">
         <v>15</v>
@@ -2788,33 +2861,33 @@
         <v>15</v>
       </c>
       <c r="H56" s="6" t="s">
-        <v>147</v>
+        <v>26</v>
       </c>
       <c r="I56" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J56" s="7">
-        <v>42095</v>
+        <v>42094</v>
       </c>
       <c r="K56" s="6" t="s">
-        <v>148</v>
+        <v>137</v>
       </c>
     </row>
     <row r="57" spans="1:11" s="6" customFormat="1" ht="24" x14ac:dyDescent="0.2">
       <c r="A57" s="6" t="s">
-        <v>149</v>
+        <v>138</v>
       </c>
       <c r="B57" s="7">
-        <v>42074</v>
+        <v>42064</v>
       </c>
       <c r="C57" s="7" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="D57" s="6" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="E57" s="6" t="s">
-        <v>54</v>
+        <v>21</v>
       </c>
       <c r="F57" s="6" t="s">
         <v>15</v>
@@ -2823,36 +2896,36 @@
         <v>15</v>
       </c>
       <c r="H57" s="6" t="s">
-        <v>17</v>
+        <v>139</v>
       </c>
       <c r="I57" s="6" t="s">
         <v>17</v>
       </c>
       <c r="J57" s="7">
-        <v>42096</v>
+        <v>42094</v>
       </c>
       <c r="K57" s="6" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="58" spans="1:11" s="6" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" s="6" customFormat="1" ht="36" x14ac:dyDescent="0.2">
       <c r="A58" s="6" t="s">
-        <v>151</v>
+        <v>141</v>
       </c>
       <c r="B58" s="7">
-        <v>42074</v>
+        <v>41709</v>
       </c>
       <c r="C58" s="7" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="D58" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E58" s="6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F58" s="6" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G58" s="6" t="s">
         <v>15</v>
@@ -2864,50 +2937,50 @@
         <v>17</v>
       </c>
       <c r="J58" s="7">
-        <v>42096</v>
+        <v>42094</v>
       </c>
       <c r="K58" s="6" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="59" spans="1:11" s="6" customFormat="1" ht="60" x14ac:dyDescent="0.2">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" s="6" customFormat="1" ht="24" x14ac:dyDescent="0.2">
       <c r="A59" s="6" t="s">
-        <v>153</v>
+        <v>143</v>
       </c>
       <c r="B59" s="7">
-        <v>42074</v>
+        <v>42064</v>
       </c>
       <c r="C59" s="7" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="D59" s="6" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="E59" s="6" t="s">
-        <v>21</v>
+        <v>52</v>
       </c>
       <c r="F59" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G59" s="6" t="s">
         <v>15</v>
       </c>
       <c r="H59" s="6" t="s">
-        <v>30</v>
+        <v>144</v>
       </c>
       <c r="I59" s="6" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="J59" s="7">
-        <v>42096</v>
+        <v>42095</v>
       </c>
       <c r="K59" s="6" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="60" spans="1:11" s="6" customFormat="1" ht="48" x14ac:dyDescent="0.2">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" s="6" customFormat="1" ht="24" x14ac:dyDescent="0.2">
       <c r="A60" s="6" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="B60" s="7">
         <v>42074</v>
@@ -2916,80 +2989,80 @@
         <v>20</v>
       </c>
       <c r="D60" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E60" s="6" t="s">
-        <v>21</v>
+        <v>52</v>
       </c>
       <c r="F60" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G60" s="6" t="s">
         <v>15</v>
       </c>
       <c r="H60" s="6" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="I60" s="6" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="J60" s="7">
         <v>42096</v>
       </c>
       <c r="K60" s="6" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="61" spans="1:11" s="6" customFormat="1" ht="60" x14ac:dyDescent="0.2">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" s="6" customFormat="1" ht="24" x14ac:dyDescent="0.2">
       <c r="A61" s="6" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
       <c r="B61" s="7">
         <v>42074</v>
       </c>
       <c r="C61" s="7" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="D61" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E61" s="6" t="s">
-        <v>37</v>
+        <v>52</v>
       </c>
       <c r="F61" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G61" s="6" t="s">
         <v>15</v>
       </c>
       <c r="H61" s="6" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="I61" s="6" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="J61" s="7">
         <v>42096</v>
       </c>
       <c r="K61" s="6" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="62" spans="1:11" s="6" customFormat="1" ht="48" x14ac:dyDescent="0.2">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" s="6" customFormat="1" ht="60" x14ac:dyDescent="0.2">
       <c r="A62" s="6" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c r="B62" s="7">
-        <v>42088</v>
-      </c>
-      <c r="C62" s="6" t="s">
+        <v>42074</v>
+      </c>
+      <c r="C62" s="7" t="s">
         <v>12</v>
       </c>
       <c r="D62" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E62" s="6" t="s">
-        <v>75</v>
+        <v>21</v>
       </c>
       <c r="F62" s="6" t="s">
         <v>16</v>
@@ -2998,30 +3071,30 @@
         <v>15</v>
       </c>
       <c r="H62" s="6" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="I62" s="6" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="J62" s="7">
         <v>42096</v>
       </c>
       <c r="K62" s="6" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="63" spans="1:11" s="6" customFormat="1" ht="60" x14ac:dyDescent="0.2">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" s="6" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A63" s="6" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="B63" s="7">
-        <v>42088</v>
-      </c>
-      <c r="C63" s="6" t="s">
-        <v>12</v>
+        <v>42074</v>
+      </c>
+      <c r="C63" s="7" t="s">
+        <v>20</v>
       </c>
       <c r="D63" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E63" s="6" t="s">
         <v>21</v>
@@ -3042,24 +3115,24 @@
         <v>42096</v>
       </c>
       <c r="K63" s="6" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="64" spans="1:11" s="6" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" s="6" customFormat="1" ht="60" x14ac:dyDescent="0.2">
       <c r="A64" s="6" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="B64" s="7">
-        <v>42093</v>
-      </c>
-      <c r="C64" s="6" t="s">
-        <v>12</v>
+        <v>42074</v>
+      </c>
+      <c r="C64" s="7" t="s">
+        <v>28</v>
       </c>
       <c r="D64" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E64" s="6" t="s">
-        <v>164</v>
+        <v>35</v>
       </c>
       <c r="F64" s="6" t="s">
         <v>16</v>
@@ -3068,33 +3141,33 @@
         <v>15</v>
       </c>
       <c r="H64" s="6" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="I64" s="6" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="J64" s="7">
         <v>42096</v>
       </c>
       <c r="K64" s="6" t="s">
-        <v>165</v>
+        <v>155</v>
       </c>
     </row>
     <row r="65" spans="1:11" s="6" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A65" s="6" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
       <c r="B65" s="7">
-        <v>42095</v>
+        <v>42088</v>
       </c>
       <c r="C65" s="6" t="s">
-        <v>29</v>
+        <v>12</v>
       </c>
       <c r="D65" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E65" s="6" t="s">
-        <v>37</v>
+        <v>72</v>
       </c>
       <c r="F65" s="6" t="s">
         <v>16</v>
@@ -3106,30 +3179,30 @@
         <v>24</v>
       </c>
       <c r="I65" s="6" t="s">
-        <v>48</v>
+        <v>22</v>
       </c>
       <c r="J65" s="7">
         <v>42096</v>
       </c>
       <c r="K65" s="6" t="s">
-        <v>167</v>
+        <v>157</v>
       </c>
     </row>
     <row r="66" spans="1:11" s="6" customFormat="1" ht="60" x14ac:dyDescent="0.2">
       <c r="A66" s="6" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
       <c r="B66" s="7">
-        <v>42092</v>
+        <v>42088</v>
       </c>
       <c r="C66" s="6" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="D66" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E66" s="6" t="s">
-        <v>37</v>
+        <v>21</v>
       </c>
       <c r="F66" s="6" t="s">
         <v>16</v>
@@ -3138,21 +3211,21 @@
         <v>15</v>
       </c>
       <c r="H66" s="6" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="I66" s="6" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="J66" s="7">
-        <v>42111</v>
+        <v>42096</v>
       </c>
       <c r="K66" s="6" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
     </row>
     <row r="67" spans="1:11" s="6" customFormat="1" ht="24" x14ac:dyDescent="0.2">
       <c r="A67" s="6" t="s">
-        <v>11</v>
+        <v>160</v>
       </c>
       <c r="B67" s="7">
         <v>42093</v>
@@ -3161,13 +3234,13 @@
         <v>12</v>
       </c>
       <c r="D67" s="6" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="E67" s="6" t="s">
-        <v>14</v>
+        <v>161</v>
       </c>
       <c r="F67" s="6" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G67" s="6" t="s">
         <v>15</v>
@@ -3179,14 +3252,450 @@
         <v>17</v>
       </c>
       <c r="J67" s="7">
+        <v>42096</v>
+      </c>
+      <c r="K67" s="6" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11" s="6" customFormat="1" ht="48" x14ac:dyDescent="0.2">
+      <c r="A68" s="6" t="s">
+        <v>163</v>
+      </c>
+      <c r="B68" s="7">
+        <v>42095</v>
+      </c>
+      <c r="C68" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D68" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="E68" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="F68" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="G68" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="H68" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="I68" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="J68" s="7">
+        <v>42096</v>
+      </c>
+      <c r="K68" s="6" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11" s="6" customFormat="1" ht="60" x14ac:dyDescent="0.2">
+      <c r="A69" s="6" t="s">
+        <v>165</v>
+      </c>
+      <c r="B69" s="7">
+        <v>42092</v>
+      </c>
+      <c r="C69" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D69" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="E69" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="F69" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="G69" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="H69" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="I69" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="J69" s="7">
+        <v>42111</v>
+      </c>
+      <c r="K69" s="6" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="70" spans="1:11" s="6" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+      <c r="A70" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B70" s="7">
+        <v>42093</v>
+      </c>
+      <c r="C70" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D70" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E70" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F70" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="G70" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="H70" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="I70" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="J70" s="7">
         <v>42115</v>
       </c>
-      <c r="K67" s="6" t="s">
+      <c r="K70" s="6" t="s">
         <v>18</v>
       </c>
     </row>
+    <row r="71" spans="1:11" s="6" customFormat="1" ht="36" x14ac:dyDescent="0.2">
+      <c r="A71" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B71" s="7">
+        <v>42073</v>
+      </c>
+      <c r="C71" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D71" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E71" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="F71" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="G71" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="H71" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="I71" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="J71" s="7">
+        <v>42156</v>
+      </c>
+      <c r="K71" s="6" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11" s="6" customFormat="1" ht="60" x14ac:dyDescent="0.2">
+      <c r="A72" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B72" s="7">
+        <v>42094</v>
+      </c>
+      <c r="C72" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D72" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E72" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="F72" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="G72" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="H72" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="I72" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="J72" s="7">
+        <v>42156</v>
+      </c>
+      <c r="K72" s="6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11" s="6" customFormat="1" ht="96" x14ac:dyDescent="0.2">
+      <c r="A73" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B73" s="7">
+        <v>42094</v>
+      </c>
+      <c r="C73" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D73" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E73" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="F73" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="G73" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="H73" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="I73" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="J73" s="7">
+        <v>42156</v>
+      </c>
+      <c r="K73" s="6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="74" spans="1:11" s="6" customFormat="1" ht="84" x14ac:dyDescent="0.2">
+      <c r="A74" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B74" s="7">
+        <v>42092</v>
+      </c>
+      <c r="C74" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D74" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="E74" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="F74" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="G74" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="H74" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="I74" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="J74" s="7">
+        <v>42156</v>
+      </c>
+      <c r="K74" s="6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="75" spans="1:11" s="6" customFormat="1" ht="96" x14ac:dyDescent="0.2">
+      <c r="A75" s="6" t="s">
+        <v>171</v>
+      </c>
+      <c r="B75" s="7">
+        <v>42113</v>
+      </c>
+      <c r="C75" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D75" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="E75" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="F75" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="G75" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="H75" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="I75" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="J75" s="7">
+        <v>42156</v>
+      </c>
+      <c r="K75" s="6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="76" spans="1:11" s="6" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+      <c r="A76" s="6" t="s">
+        <v>168</v>
+      </c>
+      <c r="B76" s="7">
+        <v>42102</v>
+      </c>
+      <c r="C76" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D76" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E76" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F76" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="G76" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="H76" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="I76" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="J76" s="7">
+        <v>42156</v>
+      </c>
+      <c r="K76" s="6" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="77" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A77" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="B77" s="7">
+        <v>42075</v>
+      </c>
+      <c r="C77" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D77" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E77" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="F77" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="G77" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="H77" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="I77" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="J77" s="7">
+        <v>42156</v>
+      </c>
+      <c r="K77" s="6" t="s">
+        <v>69</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:K41"/>
+  <autoFilter ref="A1:K44"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C13"/>
+  <sheetViews>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:C14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="60.140625" customWidth="1"/>
+    <col min="2" max="2" width="13.5703125" customWidth="1"/>
+    <col min="3" max="3" width="77.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="8"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="9"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="9"/>
+      <c r="B3" s="11"/>
+      <c r="C3" s="11"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="9"/>
+      <c r="B4" s="11"/>
+      <c r="C4" s="11"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="9"/>
+      <c r="B5" s="11"/>
+      <c r="C5" s="11"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="9"/>
+      <c r="B6" s="11"/>
+      <c r="C6" s="11"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="9"/>
+      <c r="B7" s="11"/>
+      <c r="C7" s="11"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="9"/>
+      <c r="B8" s="11"/>
+      <c r="C8" s="11"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="9"/>
+      <c r="B9" s="11"/>
+      <c r="C9" s="11"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="9"/>
+      <c r="B10" s="11"/>
+      <c r="C10" s="11"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="9"/>
+      <c r="B11" s="11"/>
+      <c r="C11" s="11"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="9"/>
+      <c r="B12" s="11"/>
+      <c r="C12" s="11"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="9"/>
+      <c r="B13" s="11"/>
+      <c r="C13" s="11"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
update doc changes plus new column for answer table
-Axe
</commit_message>
<xml_diff>
--- a/PulseBox/Documentation/PulseBox Bugs & Enhancement Requests - Master.xlsx
+++ b/PulseBox/Documentation/PulseBox Bugs & Enhancement Requests - Master.xlsx
@@ -16,7 +16,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$K$44</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$K$45</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="664" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="680" uniqueCount="206">
   <si>
     <t>Enhancement/Bug Description</t>
   </si>
@@ -219,13 +219,7 @@
     <t>As we get closer to POC, need to have data inserted which gets points across to potential customers and not just random data.</t>
   </si>
   <si>
-    <t>Location report issue</t>
-  </si>
-  <si>
     <t>Naveen/Alex</t>
-  </si>
-  <si>
-    <t>As aebadi2/6029 I added a new location for company 3005.  However this new location is not showing up Location Comparison report.  The location_id that was added is 9005.  Also, added some answers by employee 6037 for this location.</t>
   </si>
   <si>
     <t>Arch</t>
@@ -595,9 +589,6 @@
     <t>GUI</t>
   </si>
   <si>
-    <t>Need to test out multiple locations.  It was working before, but failed one time.</t>
-  </si>
-  <si>
     <t>Forecast Report - make sense of it</t>
   </si>
   <si>
@@ -665,6 +656,27 @@
   </si>
   <si>
     <t>Continue to learn from Alex, so you can start making changes to the UI and we are not always having to go to Alex.</t>
+  </si>
+  <si>
+    <t>Typo - When logging in as an employee, the top of first page says "Manager Menu"</t>
+  </si>
+  <si>
+    <t>This needs to say "Employee Menue" instead of "Manager Menu".</t>
+  </si>
+  <si>
+    <t>Need to test out multiple locations.  It was working before, but failed one time.  Added new location to company 3005 and works fine!  Just hae to remember to add right location in answer table also.</t>
+  </si>
+  <si>
+    <t>Pulse Report columns incorrect</t>
+  </si>
+  <si>
+    <t>After running Pulse Report, the columns (answer_rating, anser_dt, answer_text, dept_name) are in the wrong order!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">When I provide pulse from emp_id 6005 in company 3005 it actually ties it to question_id 13 which is part of company_id 3002!   Instead, it should tie it to question_id 16. The way it is it puts the pulse another wrong company! </t>
+  </si>
+  <si>
+    <t>Provide Pulse putting in wrong company</t>
   </si>
 </sst>
 </file>
@@ -1070,7 +1082,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K77"/>
+  <dimension ref="A1:K79"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -1130,7 +1142,7 @@
     </row>
     <row r="2" spans="1:11" s="2" customFormat="1" ht="36" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B2" s="3">
         <v>42156</v>
@@ -1151,18 +1163,18 @@
         <v>16</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="3" spans="1:11" s="2" customFormat="1" ht="24" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>176</v>
+        <v>202</v>
       </c>
       <c r="B3" s="3">
-        <v>42156</v>
+        <v>42157</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>20</v>
@@ -1171,7 +1183,7 @@
         <v>26</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>177</v>
+        <v>21</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>16</v>
@@ -1180,15 +1192,15 @@
         <v>16</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>178</v>
+        <v>203</v>
       </c>
     </row>
     <row r="4" spans="1:11" s="2" customFormat="1" ht="24" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="B4" s="3">
         <v>42156</v>
@@ -1200,27 +1212,27 @@
         <v>26</v>
       </c>
       <c r="E4" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H4" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="F4" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>180</v>
-      </c>
       <c r="K4" s="2" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" s="2" customFormat="1" ht="48" x14ac:dyDescent="0.2">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" s="2" customFormat="1" ht="36" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>198</v>
+        <v>205</v>
       </c>
       <c r="B5" s="3">
-        <v>42156</v>
+        <v>42157</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>20</v>
@@ -1238,15 +1250,15 @@
         <v>16</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>22</v>
+        <v>61</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" s="2" customFormat="1" ht="36" x14ac:dyDescent="0.2">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" s="2" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>182</v>
+        <v>195</v>
       </c>
       <c r="B6" s="3">
         <v>42156</v>
@@ -1258,7 +1270,7 @@
         <v>26</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>183</v>
+        <v>21</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>16</v>
@@ -1267,15 +1279,15 @@
         <v>16</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" s="2" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" s="2" customFormat="1" ht="36" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>188</v>
+        <v>179</v>
       </c>
       <c r="B7" s="3">
         <v>42156</v>
@@ -1287,7 +1299,7 @@
         <v>26</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>16</v>
@@ -1296,13 +1308,13 @@
         <v>16</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>102</v>
+        <v>17</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" s="2" customFormat="1" ht="36" x14ac:dyDescent="0.2">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" s="2" customFormat="1" ht="24" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>185</v>
       </c>
@@ -1316,7 +1328,7 @@
         <v>26</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>21</v>
+        <v>184</v>
       </c>
       <c r="F8" s="2" t="s">
         <v>16</v>
@@ -1325,7 +1337,7 @@
         <v>16</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>22</v>
+        <v>100</v>
       </c>
       <c r="K8" s="2" t="s">
         <v>186</v>
@@ -1333,10 +1345,10 @@
     </row>
     <row r="9" spans="1:11" s="2" customFormat="1" ht="36" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>61</v>
+        <v>182</v>
       </c>
       <c r="B9" s="3">
-        <v>42113</v>
+        <v>42156</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>20</v>
@@ -1345,7 +1357,7 @@
         <v>26</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="F9" s="2" t="s">
         <v>16</v>
@@ -1354,15 +1366,15 @@
         <v>16</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>62</v>
+        <v>22</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>63</v>
+        <v>183</v>
       </c>
     </row>
     <row r="10" spans="1:11" s="2" customFormat="1" ht="36" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="B10" s="3">
         <v>42076</v>
@@ -1386,12 +1398,12 @@
         <v>29</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
     </row>
     <row r="11" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="B11" s="3">
         <v>42156</v>
@@ -1415,12 +1427,12 @@
         <v>26</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
     </row>
     <row r="12" spans="1:11" s="2" customFormat="1" ht="24" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="B12" s="3">
         <v>42125</v>
@@ -1444,12 +1456,12 @@
         <v>17</v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
     </row>
     <row r="13" spans="1:11" s="2" customFormat="1" ht="24" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="B13" s="3">
         <v>42156</v>
@@ -1461,7 +1473,7 @@
         <v>26</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="F13" s="2" t="s">
         <v>15</v>
@@ -1470,47 +1482,47 @@
         <v>16</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" ht="48" x14ac:dyDescent="0.2">
-      <c r="A14" s="4" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" s="2" customFormat="1" ht="36" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="B14" s="3">
+        <v>42157</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="K14" s="2" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+      <c r="A15" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="B14" s="5">
+      <c r="B15" s="5">
         <v>42093</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="F14" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="G14" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="H14" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="K14" s="4" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" ht="24" x14ac:dyDescent="0.2">
-      <c r="A15" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="B15" s="5">
-        <v>42095</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>20</v>
@@ -1519,82 +1531,82 @@
         <v>26</v>
       </c>
       <c r="E15" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H15" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="K15" s="4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="24" x14ac:dyDescent="0.2">
+      <c r="A16" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" s="5">
+        <v>42095</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E16" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="F15" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="G15" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="H15" s="4" t="s">
+      <c r="F16" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G16" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H16" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="K15" s="4" t="s">
+      <c r="K16" s="4" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="36" x14ac:dyDescent="0.2">
-      <c r="A16" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="B16" s="5">
+    <row r="17" spans="1:11" ht="36" x14ac:dyDescent="0.2">
+      <c r="A17" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="B17" s="5">
         <v>42074</v>
       </c>
-      <c r="C16" s="5" t="s">
+      <c r="C17" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D16" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="E16" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="F16" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="G16" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="H16" s="4" t="s">
+      <c r="D17" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G17" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H17" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="K16" s="4" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" ht="48" x14ac:dyDescent="0.2">
-      <c r="A17" s="4" t="s">
+      <c r="K17" s="4" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+      <c r="A18" s="4" t="s">
         <v>19</v>
-      </c>
-      <c r="B17" s="5">
-        <v>42089</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E17" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="F17" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="G17" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="H17" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="K17" s="4" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" ht="36" x14ac:dyDescent="0.2">
-      <c r="A18" s="4" t="s">
-        <v>45</v>
       </c>
       <c r="B18" s="5">
         <v>42089</v>
@@ -1603,10 +1615,10 @@
         <v>12</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>46</v>
+        <v>13</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>47</v>
+        <v>21</v>
       </c>
       <c r="F18" s="4" t="s">
         <v>15</v>
@@ -1615,18 +1627,18 @@
         <v>16</v>
       </c>
       <c r="H18" s="4" t="s">
-        <v>46</v>
+        <v>22</v>
       </c>
       <c r="K18" s="4" t="s">
-        <v>48</v>
+        <v>165</v>
       </c>
     </row>
     <row r="19" spans="1:11" ht="36" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B19" s="5">
-        <v>42096</v>
+        <v>42089</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>12</v>
@@ -1635,7 +1647,7 @@
         <v>46</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>21</v>
+        <v>47</v>
       </c>
       <c r="F19" s="4" t="s">
         <v>15</v>
@@ -1644,44 +1656,44 @@
         <v>16</v>
       </c>
       <c r="H19" s="4" t="s">
-        <v>22</v>
+        <v>46</v>
       </c>
       <c r="K19" s="4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="20" spans="1:11" ht="36" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B20" s="5">
-        <v>42113</v>
+        <v>42096</v>
       </c>
       <c r="C20" s="4" t="s">
         <v>12</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>26</v>
+        <v>46</v>
       </c>
       <c r="E20" s="4" t="s">
         <v>21</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G20" s="4" t="s">
         <v>16</v>
       </c>
       <c r="H20" s="4" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="K20" s="4" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" ht="60" x14ac:dyDescent="0.2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="36" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B21" s="5">
         <v>42113</v>
@@ -1705,12 +1717,12 @@
         <v>17</v>
       </c>
       <c r="K21" s="4" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" ht="24" x14ac:dyDescent="0.2">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" ht="60" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B22" s="5">
         <v>42113</v>
@@ -1722,7 +1734,7 @@
         <v>26</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="F22" s="4" t="s">
         <v>16</v>
@@ -1734,27 +1746,27 @@
         <v>17</v>
       </c>
       <c r="K22" s="4" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="23" spans="1:11" ht="24" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
-        <v>41</v>
+        <v>57</v>
       </c>
       <c r="B23" s="5">
-        <v>42064</v>
-      </c>
-      <c r="C23" s="5" t="s">
+        <v>42113</v>
+      </c>
+      <c r="C23" s="4" t="s">
         <v>12</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>21</v>
+        <v>35</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G23" s="4" t="s">
         <v>16</v>
@@ -1763,140 +1775,140 @@
         <v>17</v>
       </c>
       <c r="K23" s="4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" ht="24" x14ac:dyDescent="0.2">
+      <c r="A24" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B24" s="5">
+        <v>42064</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F24" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G24" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H24" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="K24" s="4" t="s">
         <v>42</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" ht="36" x14ac:dyDescent="0.2">
-      <c r="A24" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="B24" s="5">
-        <v>42113</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D24" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="E24" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="F24" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="G24" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="H24" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="K24" s="4" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="25" spans="1:11" ht="36" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B25" s="5">
+        <v>42113</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="F25" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G25" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H25" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="K25" s="4" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" ht="36" x14ac:dyDescent="0.2">
+      <c r="A26" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B25" s="5">
+      <c r="B26" s="5">
         <v>42074</v>
       </c>
-      <c r="C25" s="5" t="s">
+      <c r="C26" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D25" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="E25" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="F25" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="G25" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="H25" s="4" t="s">
+      <c r="D26" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E26" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F26" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G26" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H26" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="K25" s="4" t="s">
+      <c r="K26" s="4" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="26" spans="1:11" ht="48" x14ac:dyDescent="0.2">
-      <c r="A26" s="4" t="s">
+    <row r="27" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+      <c r="A27" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="B26" s="5">
+      <c r="B27" s="5">
         <v>42113</v>
-      </c>
-      <c r="C26" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D26" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="E26" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="F26" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="G26" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="H26" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="K26" s="4" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" ht="36" x14ac:dyDescent="0.2">
-      <c r="A27" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="B27" s="5">
-        <v>42088</v>
       </c>
       <c r="C27" s="4" t="s">
         <v>12</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>71</v>
+        <v>26</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>72</v>
+        <v>52</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G27" s="4" t="s">
         <v>16</v>
       </c>
       <c r="H27" s="4" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="K27" s="4" t="s">
-        <v>73</v>
+        <v>168</v>
       </c>
     </row>
     <row r="28" spans="1:11" ht="36" x14ac:dyDescent="0.2">
       <c r="A28" s="4" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="B28" s="5">
         <v>42088</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>22</v>
+        <v>69</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="F28" s="4" t="s">
         <v>15</v>
@@ -1905,123 +1917,117 @@
         <v>16</v>
       </c>
       <c r="H28" s="4" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="K28" s="4" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
     </row>
     <row r="29" spans="1:11" ht="36" x14ac:dyDescent="0.2">
       <c r="A29" s="4" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="B29" s="5">
+        <v>42088</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E29" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="F29" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G29" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H29" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="K29" s="4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" ht="36" x14ac:dyDescent="0.2">
+      <c r="A30" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="B30" s="5">
         <v>42093</v>
-      </c>
-      <c r="C29" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D29" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="E29" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="F29" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="G29" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="H29" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="K29" s="4" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A30" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="B30" s="5">
-        <v>42096</v>
       </c>
       <c r="C30" s="4" t="s">
         <v>12</v>
       </c>
       <c r="D30" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E30" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F30" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G30" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H30" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="K30" s="4" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A31" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="B31" s="5">
+        <v>42096</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D31" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="E30" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="F30" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="G30" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="H30" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="K30" s="4" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" s="6" customFormat="1" ht="36" x14ac:dyDescent="0.2">
-      <c r="A31" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="B31" s="7">
+      <c r="E31" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F31" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G31" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H31" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="K31" s="4" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" s="6" customFormat="1" ht="36" x14ac:dyDescent="0.2">
+      <c r="A32" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="B32" s="7">
         <v>42073</v>
-      </c>
-      <c r="C31" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="D31" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="E31" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="F31" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="G31" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="H31" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="I31" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="J31" s="7">
-        <v>42087</v>
-      </c>
-      <c r="K31" s="6" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11" s="6" customFormat="1" ht="24" x14ac:dyDescent="0.2">
-      <c r="A32" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="B32" s="7">
-        <v>42064</v>
       </c>
       <c r="C32" s="7" t="s">
         <v>28</v>
       </c>
       <c r="D32" s="6" t="s">
-        <v>26</v>
+        <v>80</v>
       </c>
       <c r="E32" s="6" t="s">
         <v>21</v>
       </c>
       <c r="F32" s="6" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G32" s="6" t="s">
         <v>15</v>
@@ -2033,27 +2039,27 @@
         <v>22</v>
       </c>
       <c r="J32" s="7">
-        <v>42075</v>
+        <v>42087</v>
       </c>
       <c r="K32" s="6" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="33" spans="1:11" s="6" customFormat="1" ht="96" x14ac:dyDescent="0.2">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" s="6" customFormat="1" ht="24" x14ac:dyDescent="0.2">
       <c r="A33" s="6" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="B33" s="7">
-        <v>42073</v>
+        <v>42064</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="D33" s="6" t="s">
         <v>26</v>
       </c>
       <c r="E33" s="6" t="s">
-        <v>87</v>
+        <v>21</v>
       </c>
       <c r="F33" s="6" t="s">
         <v>15</v>
@@ -2062,33 +2068,33 @@
         <v>15</v>
       </c>
       <c r="H33" s="6" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="I33" s="6" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="J33" s="7">
         <v>42075</v>
       </c>
       <c r="K33" s="6" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="34" spans="1:11" s="6" customFormat="1" ht="36" x14ac:dyDescent="0.2">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" s="6" customFormat="1" ht="96" x14ac:dyDescent="0.2">
       <c r="A34" s="6" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="B34" s="7">
         <v>42073</v>
       </c>
       <c r="C34" s="7" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="D34" s="6" t="s">
         <v>26</v>
       </c>
       <c r="E34" s="6" t="s">
-        <v>21</v>
+        <v>85</v>
       </c>
       <c r="F34" s="6" t="s">
         <v>15</v>
@@ -2097,21 +2103,21 @@
         <v>15</v>
       </c>
       <c r="H34" s="6" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="I34" s="6" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="J34" s="7">
-        <v>42076</v>
+        <v>42075</v>
       </c>
       <c r="K34" s="6" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="35" spans="1:11" s="6" customFormat="1" ht="60" x14ac:dyDescent="0.2">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" s="6" customFormat="1" ht="36" x14ac:dyDescent="0.2">
       <c r="A35" s="6" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="B35" s="7">
         <v>42073</v>
@@ -2126,68 +2132,68 @@
         <v>21</v>
       </c>
       <c r="F35" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G35" s="6" t="s">
         <v>15</v>
       </c>
       <c r="H35" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="I35" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="J35" s="7">
+        <v>42076</v>
+      </c>
+      <c r="K35" s="6" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" s="6" customFormat="1" ht="60" x14ac:dyDescent="0.2">
+      <c r="A36" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="B36" s="7">
+        <v>42073</v>
+      </c>
+      <c r="C36" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D36" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="E36" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="F36" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="G36" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="H36" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="J35" s="7">
+      <c r="J36" s="7">
         <v>42088</v>
       </c>
-      <c r="K35" s="6" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="36" spans="1:11" s="6" customFormat="1" ht="24" x14ac:dyDescent="0.2">
-      <c r="A36" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="B36" s="7">
+      <c r="K36" s="6" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" s="6" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+      <c r="A37" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="B37" s="7">
         <v>42064</v>
-      </c>
-      <c r="C36" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="D36" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="E36" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="F36" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="G36" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="H36" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="I36" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="J36" s="7">
-        <v>42075</v>
-      </c>
-      <c r="K36" s="6" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="37" spans="1:11" s="6" customFormat="1" ht="72" x14ac:dyDescent="0.2">
-      <c r="A37" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="B37" s="7">
-        <v>42073</v>
       </c>
       <c r="C37" s="7" t="s">
         <v>20</v>
       </c>
       <c r="D37" s="6" t="s">
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="E37" s="6" t="s">
         <v>21</v>
@@ -2205,100 +2211,100 @@
         <v>22</v>
       </c>
       <c r="J37" s="7">
-        <v>42087</v>
+        <v>42075</v>
       </c>
       <c r="K37" s="6" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="38" spans="1:11" s="6" customFormat="1" ht="93.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" s="6" customFormat="1" ht="72" x14ac:dyDescent="0.2">
       <c r="A38" s="6" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="B38" s="7">
-        <v>42074</v>
+        <v>42073</v>
       </c>
       <c r="C38" s="7" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="D38" s="6" t="s">
         <v>26</v>
       </c>
       <c r="E38" s="6" t="s">
-        <v>47</v>
+        <v>21</v>
       </c>
       <c r="F38" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G38" s="6" t="s">
         <v>15</v>
       </c>
       <c r="H38" s="6" t="s">
-        <v>46</v>
+        <v>22</v>
       </c>
       <c r="I38" s="6" t="s">
-        <v>46</v>
+        <v>22</v>
       </c>
       <c r="J38" s="7">
         <v>42087</v>
       </c>
       <c r="K38" s="6" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="39" spans="1:11" s="6" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" s="6" customFormat="1" ht="93.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="6" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="B39" s="7">
+        <v>42074</v>
+      </c>
+      <c r="C39" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D39" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="E39" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="F39" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="G39" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="H39" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="I39" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="J39" s="7">
+        <v>42087</v>
+      </c>
+      <c r="K39" s="6" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" s="6" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+      <c r="A40" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="B40" s="7">
         <v>42075</v>
-      </c>
-      <c r="C39" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="D39" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="E39" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="F39" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="G39" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="H39" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="I39" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="J39" s="7">
-        <v>42075</v>
-      </c>
-      <c r="K39" s="6" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="40" spans="1:11" s="6" customFormat="1" ht="36" x14ac:dyDescent="0.2">
-      <c r="A40" s="6" t="s">
-        <v>101</v>
-      </c>
-      <c r="B40" s="7">
-        <v>42080</v>
       </c>
       <c r="C40" s="7" t="s">
         <v>20</v>
       </c>
       <c r="D40" s="6" t="s">
-        <v>102</v>
+        <v>13</v>
       </c>
       <c r="E40" s="6" t="s">
-        <v>72</v>
+        <v>21</v>
       </c>
       <c r="F40" s="6" t="s">
-        <v>103</v>
+        <v>15</v>
       </c>
       <c r="G40" s="6" t="s">
         <v>15</v>
@@ -2310,65 +2316,65 @@
         <v>22</v>
       </c>
       <c r="J40" s="7">
-        <v>42087</v>
+        <v>42075</v>
       </c>
       <c r="K40" s="6" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="41" spans="1:11" s="6" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" s="6" customFormat="1" ht="36" x14ac:dyDescent="0.2">
       <c r="A41" s="6" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="B41" s="7">
         <v>42080</v>
       </c>
       <c r="C41" s="7" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="D41" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="E41" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="F41" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="G41" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="H41" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="I41" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="J41" s="7">
+        <v>42087</v>
+      </c>
+      <c r="K41" s="6" t="s">
         <v>102</v>
-      </c>
-      <c r="E41" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="F41" s="6" t="s">
-        <v>103</v>
-      </c>
-      <c r="G41" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="H41" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="I41" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="J41" s="7">
-        <v>42089</v>
-      </c>
-      <c r="K41" s="6" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="42" spans="1:11" s="6" customFormat="1" ht="24" x14ac:dyDescent="0.2">
       <c r="A42" s="6" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="B42" s="7">
-        <v>42088</v>
-      </c>
-      <c r="C42" s="6" t="s">
-        <v>20</v>
+        <v>42080</v>
+      </c>
+      <c r="C42" s="7" t="s">
+        <v>12</v>
       </c>
       <c r="D42" s="6" t="s">
-        <v>26</v>
+        <v>100</v>
       </c>
       <c r="E42" s="6" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F42" s="6" t="s">
-        <v>15</v>
+        <v>101</v>
       </c>
       <c r="G42" s="6" t="s">
         <v>15</v>
@@ -2383,12 +2389,12 @@
         <v>42089</v>
       </c>
       <c r="K42" s="6" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
     </row>
     <row r="43" spans="1:11" s="6" customFormat="1" ht="24" x14ac:dyDescent="0.2">
       <c r="A43" s="6" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="B43" s="7">
         <v>42088</v>
@@ -2400,10 +2406,10 @@
         <v>26</v>
       </c>
       <c r="E43" s="6" t="s">
-        <v>21</v>
+        <v>70</v>
       </c>
       <c r="F43" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G43" s="6" t="s">
         <v>15</v>
@@ -2418,12 +2424,12 @@
         <v>42089</v>
       </c>
       <c r="K43" s="6" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
     </row>
     <row r="44" spans="1:11" s="6" customFormat="1" ht="24" x14ac:dyDescent="0.2">
       <c r="A44" s="6" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="B44" s="7">
         <v>42088</v>
@@ -2432,13 +2438,13 @@
         <v>20</v>
       </c>
       <c r="D44" s="6" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="E44" s="6" t="s">
         <v>21</v>
       </c>
       <c r="F44" s="6" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G44" s="6" t="s">
         <v>15</v>
@@ -2453,56 +2459,56 @@
         <v>42089</v>
       </c>
       <c r="K44" s="6" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
     </row>
     <row r="45" spans="1:11" s="6" customFormat="1" ht="24" x14ac:dyDescent="0.2">
       <c r="A45" s="6" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="B45" s="7">
+        <v>42088</v>
+      </c>
+      <c r="C45" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D45" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E45" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="F45" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="G45" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="H45" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="I45" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="J45" s="7">
+        <v>42089</v>
+      </c>
+      <c r="K45" s="6" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" s="6" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+      <c r="A46" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="B46" s="7">
         <v>42073</v>
       </c>
-      <c r="C45" s="7" t="s">
+      <c r="C46" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="D45" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="E45" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="F45" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="G45" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="H45" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="I45" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="J45" s="7">
-        <v>42091</v>
-      </c>
-      <c r="K45" s="6" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="46" spans="1:11" s="6" customFormat="1" ht="36" x14ac:dyDescent="0.2">
-      <c r="A46" s="6" t="s">
-        <v>115</v>
-      </c>
-      <c r="B46" s="7">
-        <v>42074</v>
-      </c>
-      <c r="C46" s="7" t="s">
-        <v>12</v>
-      </c>
       <c r="D46" s="6" t="s">
-        <v>26</v>
+        <v>80</v>
       </c>
       <c r="E46" s="6" t="s">
         <v>21</v>
@@ -2523,12 +2529,12 @@
         <v>42091</v>
       </c>
       <c r="K46" s="6" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="47" spans="1:11" s="6" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" s="6" customFormat="1" ht="36" x14ac:dyDescent="0.2">
       <c r="A47" s="6" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="B47" s="7">
         <v>42074</v>
@@ -2558,27 +2564,27 @@
         <v>42091</v>
       </c>
       <c r="K47" s="6" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="48" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.2">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" s="6" customFormat="1" ht="24" x14ac:dyDescent="0.2">
       <c r="A48" s="6" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="B48" s="7">
-        <v>42088</v>
-      </c>
-      <c r="C48" s="6" t="s">
-        <v>20</v>
+        <v>42074</v>
+      </c>
+      <c r="C48" s="7" t="s">
+        <v>12</v>
       </c>
       <c r="D48" s="6" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="E48" s="6" t="s">
-        <v>72</v>
+        <v>21</v>
       </c>
       <c r="F48" s="6" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G48" s="6" t="s">
         <v>15</v>
@@ -2593,24 +2599,24 @@
         <v>42091</v>
       </c>
       <c r="K48" s="6" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="49" spans="1:11" s="6" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A49" s="6" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="B49" s="7">
         <v>42088</v>
       </c>
       <c r="C49" s="6" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="D49" s="6" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="E49" s="6" t="s">
-        <v>47</v>
+        <v>70</v>
       </c>
       <c r="F49" s="6" t="s">
         <v>15</v>
@@ -2628,27 +2634,27 @@
         <v>42091</v>
       </c>
       <c r="K49" s="6" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="50" spans="1:11" s="6" customFormat="1" ht="24" x14ac:dyDescent="0.2">
       <c r="A50" s="6" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="B50" s="7">
         <v>42088</v>
       </c>
       <c r="C50" s="6" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="D50" s="6" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="E50" s="6" t="s">
-        <v>21</v>
+        <v>47</v>
       </c>
       <c r="F50" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G50" s="6" t="s">
         <v>15</v>
@@ -2663,18 +2669,18 @@
         <v>42091</v>
       </c>
       <c r="K50" s="6" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="51" spans="1:11" s="6" customFormat="1" ht="48" x14ac:dyDescent="0.2">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" s="6" customFormat="1" ht="24" x14ac:dyDescent="0.2">
       <c r="A51" s="6" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="B51" s="7">
-        <v>42073</v>
-      </c>
-      <c r="C51" s="7" t="s">
-        <v>12</v>
+        <v>42088</v>
+      </c>
+      <c r="C51" s="6" t="s">
+        <v>20</v>
       </c>
       <c r="D51" s="6" t="s">
         <v>26</v>
@@ -2689,18 +2695,21 @@
         <v>15</v>
       </c>
       <c r="H51" s="6" t="s">
-        <v>13</v>
+        <v>22</v>
+      </c>
+      <c r="I51" s="6" t="s">
+        <v>22</v>
       </c>
       <c r="J51" s="7">
-        <v>42092</v>
+        <v>42091</v>
       </c>
       <c r="K51" s="6" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="52" spans="1:11" s="6" customFormat="1" ht="84" x14ac:dyDescent="0.2">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" s="6" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A52" s="6" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="B52" s="7">
         <v>42073</v>
@@ -2709,7 +2718,7 @@
         <v>12</v>
       </c>
       <c r="D52" s="6" t="s">
-        <v>82</v>
+        <v>26</v>
       </c>
       <c r="E52" s="6" t="s">
         <v>21</v>
@@ -2721,138 +2730,135 @@
         <v>15</v>
       </c>
       <c r="H52" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="I52" s="6" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="J52" s="7">
         <v>42092</v>
       </c>
       <c r="K52" s="6" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="53" spans="1:11" s="6" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" s="6" customFormat="1" ht="84" x14ac:dyDescent="0.2">
       <c r="A53" s="6" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="B53" s="7">
-        <v>42088</v>
-      </c>
-      <c r="C53" s="6" t="s">
-        <v>20</v>
+        <v>42073</v>
+      </c>
+      <c r="C53" s="7" t="s">
+        <v>12</v>
       </c>
       <c r="D53" s="6" t="s">
-        <v>26</v>
+        <v>80</v>
       </c>
       <c r="E53" s="6" t="s">
-        <v>47</v>
+        <v>21</v>
       </c>
       <c r="F53" s="6" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G53" s="6" t="s">
         <v>15</v>
       </c>
       <c r="H53" s="6" t="s">
-        <v>46</v>
+        <v>22</v>
       </c>
       <c r="I53" s="6" t="s">
-        <v>46</v>
+        <v>22</v>
       </c>
       <c r="J53" s="7">
         <v>42092</v>
       </c>
       <c r="K53" s="6" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="54" spans="1:11" s="6" customFormat="1" ht="120" x14ac:dyDescent="0.2">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" s="6" customFormat="1" ht="24" x14ac:dyDescent="0.2">
       <c r="A54" s="6" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="B54" s="7">
         <v>42088</v>
       </c>
       <c r="C54" s="6" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="D54" s="6" t="s">
         <v>26</v>
       </c>
       <c r="E54" s="6" t="s">
-        <v>35</v>
+        <v>47</v>
       </c>
       <c r="F54" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G54" s="6" t="s">
         <v>15</v>
       </c>
       <c r="H54" s="6" t="s">
-        <v>24</v>
+        <v>46</v>
       </c>
       <c r="I54" s="6" t="s">
         <v>46</v>
       </c>
       <c r="J54" s="7">
-        <v>42093</v>
+        <v>42092</v>
       </c>
       <c r="K54" s="6" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="55" spans="1:11" s="6" customFormat="1" ht="36" x14ac:dyDescent="0.2">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" s="6" customFormat="1" ht="120" x14ac:dyDescent="0.2">
       <c r="A55" s="6" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="B55" s="7">
         <v>42088</v>
       </c>
       <c r="C55" s="6" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="D55" s="6" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="E55" s="6" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="F55" s="6" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G55" s="6" t="s">
         <v>15</v>
       </c>
       <c r="H55" s="6" t="s">
-        <v>46</v>
+        <v>24</v>
       </c>
       <c r="I55" s="6" t="s">
         <v>46</v>
       </c>
       <c r="J55" s="7">
-        <v>42094</v>
+        <v>42093</v>
       </c>
       <c r="K55" s="6" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="56" spans="1:11" s="6" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" s="6" customFormat="1" ht="36" x14ac:dyDescent="0.2">
       <c r="A56" s="6" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="B56" s="7">
         <v>42088</v>
       </c>
       <c r="C56" s="6" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="D56" s="6" t="s">
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="E56" s="6" t="s">
-        <v>136</v>
+        <v>47</v>
       </c>
       <c r="F56" s="6" t="s">
         <v>15</v>
@@ -2861,33 +2867,33 @@
         <v>15</v>
       </c>
       <c r="H56" s="6" t="s">
-        <v>26</v>
+        <v>46</v>
       </c>
       <c r="I56" s="6" t="s">
-        <v>26</v>
+        <v>46</v>
       </c>
       <c r="J56" s="7">
         <v>42094</v>
       </c>
       <c r="K56" s="6" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
     </row>
     <row r="57" spans="1:11" s="6" customFormat="1" ht="24" x14ac:dyDescent="0.2">
       <c r="A57" s="6" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="B57" s="7">
-        <v>42064</v>
-      </c>
-      <c r="C57" s="7" t="s">
-        <v>12</v>
+        <v>42088</v>
+      </c>
+      <c r="C57" s="6" t="s">
+        <v>28</v>
       </c>
       <c r="D57" s="6" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="E57" s="6" t="s">
-        <v>21</v>
+        <v>134</v>
       </c>
       <c r="F57" s="6" t="s">
         <v>15</v>
@@ -2896,42 +2902,42 @@
         <v>15</v>
       </c>
       <c r="H57" s="6" t="s">
-        <v>139</v>
+        <v>26</v>
       </c>
       <c r="I57" s="6" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="J57" s="7">
         <v>42094</v>
       </c>
       <c r="K57" s="6" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="58" spans="1:11" s="6" customFormat="1" ht="36" x14ac:dyDescent="0.2">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" s="6" customFormat="1" ht="24" x14ac:dyDescent="0.2">
       <c r="A58" s="6" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="B58" s="7">
-        <v>41709</v>
+        <v>42064</v>
       </c>
       <c r="C58" s="7" t="s">
         <v>12</v>
       </c>
       <c r="D58" s="6" t="s">
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="E58" s="6" t="s">
-        <v>52</v>
+        <v>21</v>
       </c>
       <c r="F58" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G58" s="6" t="s">
         <v>15</v>
       </c>
       <c r="H58" s="6" t="s">
-        <v>17</v>
+        <v>137</v>
       </c>
       <c r="I58" s="6" t="s">
         <v>17</v>
@@ -2940,56 +2946,56 @@
         <v>42094</v>
       </c>
       <c r="K58" s="6" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="59" spans="1:11" s="6" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" s="6" customFormat="1" ht="36" x14ac:dyDescent="0.2">
       <c r="A59" s="6" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="B59" s="7">
-        <v>42064</v>
+        <v>41709</v>
       </c>
       <c r="C59" s="7" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="D59" s="6" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="E59" s="6" t="s">
         <v>52</v>
       </c>
       <c r="F59" s="6" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G59" s="6" t="s">
         <v>15</v>
       </c>
       <c r="H59" s="6" t="s">
-        <v>144</v>
+        <v>17</v>
       </c>
       <c r="I59" s="6" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="J59" s="7">
-        <v>42095</v>
+        <v>42094</v>
       </c>
       <c r="K59" s="6" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
     </row>
     <row r="60" spans="1:11" s="6" customFormat="1" ht="24" x14ac:dyDescent="0.2">
       <c r="A60" s="6" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="B60" s="7">
-        <v>42074</v>
+        <v>42064</v>
       </c>
       <c r="C60" s="7" t="s">
         <v>20</v>
       </c>
       <c r="D60" s="6" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="E60" s="6" t="s">
         <v>52</v>
@@ -3001,21 +3007,21 @@
         <v>15</v>
       </c>
       <c r="H60" s="6" t="s">
-        <v>17</v>
+        <v>142</v>
       </c>
       <c r="I60" s="6" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="J60" s="7">
-        <v>42096</v>
+        <v>42095</v>
       </c>
       <c r="K60" s="6" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
     </row>
     <row r="61" spans="1:11" s="6" customFormat="1" ht="24" x14ac:dyDescent="0.2">
       <c r="A61" s="6" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="B61" s="7">
         <v>42074</v>
@@ -3045,53 +3051,53 @@
         <v>42096</v>
       </c>
       <c r="K61" s="6" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="62" spans="1:11" s="6" customFormat="1" ht="60" x14ac:dyDescent="0.2">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" s="6" customFormat="1" ht="24" x14ac:dyDescent="0.2">
       <c r="A62" s="6" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="B62" s="7">
         <v>42074</v>
       </c>
       <c r="C62" s="7" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="D62" s="6" t="s">
         <v>26</v>
       </c>
       <c r="E62" s="6" t="s">
-        <v>21</v>
+        <v>52</v>
       </c>
       <c r="F62" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G62" s="6" t="s">
         <v>15</v>
       </c>
       <c r="H62" s="6" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="I62" s="6" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="J62" s="7">
         <v>42096</v>
       </c>
       <c r="K62" s="6" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="63" spans="1:11" s="6" customFormat="1" ht="48" x14ac:dyDescent="0.2">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" s="6" customFormat="1" ht="60" x14ac:dyDescent="0.2">
       <c r="A63" s="6" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="B63" s="7">
         <v>42074</v>
       </c>
       <c r="C63" s="7" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="D63" s="6" t="s">
         <v>26</v>
@@ -3106,33 +3112,33 @@
         <v>15</v>
       </c>
       <c r="H63" s="6" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="I63" s="6" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="J63" s="7">
         <v>42096</v>
       </c>
       <c r="K63" s="6" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="64" spans="1:11" s="6" customFormat="1" ht="60" x14ac:dyDescent="0.2">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" s="6" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A64" s="6" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="B64" s="7">
         <v>42074</v>
       </c>
       <c r="C64" s="7" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="D64" s="6" t="s">
         <v>26</v>
       </c>
       <c r="E64" s="6" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="F64" s="6" t="s">
         <v>16</v>
@@ -3141,7 +3147,7 @@
         <v>15</v>
       </c>
       <c r="H64" s="6" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="I64" s="6" t="s">
         <v>22</v>
@@ -3150,24 +3156,24 @@
         <v>42096</v>
       </c>
       <c r="K64" s="6" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="65" spans="1:11" s="6" customFormat="1" ht="48" x14ac:dyDescent="0.2">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11" s="6" customFormat="1" ht="60" x14ac:dyDescent="0.2">
       <c r="A65" s="6" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="B65" s="7">
-        <v>42088</v>
-      </c>
-      <c r="C65" s="6" t="s">
-        <v>12</v>
+        <v>42074</v>
+      </c>
+      <c r="C65" s="7" t="s">
+        <v>28</v>
       </c>
       <c r="D65" s="6" t="s">
         <v>26</v>
       </c>
       <c r="E65" s="6" t="s">
-        <v>72</v>
+        <v>35</v>
       </c>
       <c r="F65" s="6" t="s">
         <v>16</v>
@@ -3185,12 +3191,12 @@
         <v>42096</v>
       </c>
       <c r="K65" s="6" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="66" spans="1:11" s="6" customFormat="1" ht="60" x14ac:dyDescent="0.2">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11" s="6" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A66" s="6" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="B66" s="7">
         <v>42088</v>
@@ -3202,7 +3208,7 @@
         <v>26</v>
       </c>
       <c r="E66" s="6" t="s">
-        <v>21</v>
+        <v>70</v>
       </c>
       <c r="F66" s="6" t="s">
         <v>16</v>
@@ -3211,7 +3217,7 @@
         <v>15</v>
       </c>
       <c r="H66" s="6" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="I66" s="6" t="s">
         <v>22</v>
@@ -3220,15 +3226,15 @@
         <v>42096</v>
       </c>
       <c r="K66" s="6" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="67" spans="1:11" s="6" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11" s="6" customFormat="1" ht="60" x14ac:dyDescent="0.2">
       <c r="A67" s="6" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="B67" s="7">
-        <v>42093</v>
+        <v>42088</v>
       </c>
       <c r="C67" s="6" t="s">
         <v>12</v>
@@ -3237,7 +3243,7 @@
         <v>26</v>
       </c>
       <c r="E67" s="6" t="s">
-        <v>161</v>
+        <v>21</v>
       </c>
       <c r="F67" s="6" t="s">
         <v>16</v>
@@ -3246,33 +3252,33 @@
         <v>15</v>
       </c>
       <c r="H67" s="6" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="I67" s="6" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="J67" s="7">
         <v>42096</v>
       </c>
       <c r="K67" s="6" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="68" spans="1:11" s="6" customFormat="1" ht="48" x14ac:dyDescent="0.2">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11" s="6" customFormat="1" ht="24" x14ac:dyDescent="0.2">
       <c r="A68" s="6" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="B68" s="7">
-        <v>42095</v>
+        <v>42093</v>
       </c>
       <c r="C68" s="6" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
       <c r="D68" s="6" t="s">
         <v>26</v>
       </c>
       <c r="E68" s="6" t="s">
-        <v>35</v>
+        <v>159</v>
       </c>
       <c r="F68" s="6" t="s">
         <v>16</v>
@@ -3281,27 +3287,27 @@
         <v>15</v>
       </c>
       <c r="H68" s="6" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="I68" s="6" t="s">
-        <v>46</v>
+        <v>17</v>
       </c>
       <c r="J68" s="7">
         <v>42096</v>
       </c>
       <c r="K68" s="6" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="69" spans="1:11" s="6" customFormat="1" ht="60" x14ac:dyDescent="0.2">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11" s="6" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A69" s="6" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="B69" s="7">
-        <v>42092</v>
+        <v>42095</v>
       </c>
       <c r="C69" s="6" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="D69" s="6" t="s">
         <v>26</v>
@@ -3319,65 +3325,65 @@
         <v>24</v>
       </c>
       <c r="I69" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="J69" s="7">
+        <v>42096</v>
+      </c>
+      <c r="K69" s="6" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="70" spans="1:11" s="6" customFormat="1" ht="60" x14ac:dyDescent="0.2">
+      <c r="A70" s="6" t="s">
+        <v>163</v>
+      </c>
+      <c r="B70" s="7">
+        <v>42092</v>
+      </c>
+      <c r="C70" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D70" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="E70" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="F70" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="G70" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="H70" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="I70" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="J69" s="7">
+      <c r="J70" s="7">
         <v>42111</v>
       </c>
-      <c r="K69" s="6" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="70" spans="1:11" s="6" customFormat="1" ht="24" x14ac:dyDescent="0.2">
-      <c r="A70" s="6" t="s">
+      <c r="K70" s="6" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="71" spans="1:11" s="6" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+      <c r="A71" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="B70" s="7">
+      <c r="B71" s="7">
         <v>42093</v>
       </c>
-      <c r="C70" s="6" t="s">
+      <c r="C71" s="6" t="s">
         <v>12</v>
-      </c>
-      <c r="D70" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="E70" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="F70" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="G70" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="H70" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="I70" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="J70" s="7">
-        <v>42115</v>
-      </c>
-      <c r="K70" s="6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="71" spans="1:11" s="6" customFormat="1" ht="36" x14ac:dyDescent="0.2">
-      <c r="A71" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="B71" s="7">
-        <v>42073</v>
-      </c>
-      <c r="C71" s="7" t="s">
-        <v>28</v>
       </c>
       <c r="D71" s="6" t="s">
         <v>13</v>
       </c>
       <c r="E71" s="6" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="F71" s="6" t="s">
         <v>15</v>
@@ -3386,30 +3392,30 @@
         <v>15</v>
       </c>
       <c r="H71" s="6" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="I71" s="6" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="J71" s="7">
-        <v>42156</v>
+        <v>42115</v>
       </c>
       <c r="K71" s="6" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="72" spans="1:11" s="6" customFormat="1" ht="60" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11" s="6" customFormat="1" ht="36" x14ac:dyDescent="0.2">
       <c r="A72" s="6" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="B72" s="7">
-        <v>42094</v>
-      </c>
-      <c r="C72" s="6" t="s">
+        <v>42073</v>
+      </c>
+      <c r="C72" s="7" t="s">
         <v>28</v>
       </c>
       <c r="D72" s="6" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="E72" s="6" t="s">
         <v>21</v>
@@ -3421,33 +3427,33 @@
         <v>15</v>
       </c>
       <c r="H72" s="6" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="I72" s="6" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="J72" s="7">
         <v>42156</v>
       </c>
       <c r="K72" s="6" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="73" spans="1:11" s="6" customFormat="1" ht="96" x14ac:dyDescent="0.2">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11" s="6" customFormat="1" ht="60" x14ac:dyDescent="0.2">
       <c r="A73" s="6" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="B73" s="7">
         <v>42094</v>
       </c>
       <c r="C73" s="6" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="D73" s="6" t="s">
         <v>22</v>
       </c>
       <c r="E73" s="6" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="F73" s="6" t="s">
         <v>15</v>
@@ -3465,27 +3471,27 @@
         <v>42156</v>
       </c>
       <c r="K73" s="6" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="74" spans="1:11" s="6" customFormat="1" ht="84" x14ac:dyDescent="0.2">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="74" spans="1:11" s="6" customFormat="1" ht="96" x14ac:dyDescent="0.2">
       <c r="A74" s="6" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B74" s="7">
-        <v>42092</v>
+        <v>42094</v>
       </c>
       <c r="C74" s="6" t="s">
         <v>20</v>
       </c>
       <c r="D74" s="6" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="E74" s="6" t="s">
-        <v>21</v>
+        <v>35</v>
       </c>
       <c r="F74" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G74" s="6" t="s">
         <v>15</v>
@@ -3500,24 +3506,24 @@
         <v>42156</v>
       </c>
       <c r="K74" s="6" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="75" spans="1:11" s="6" customFormat="1" ht="96" x14ac:dyDescent="0.2">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="75" spans="1:11" s="6" customFormat="1" ht="84" x14ac:dyDescent="0.2">
       <c r="A75" s="6" t="s">
-        <v>171</v>
+        <v>39</v>
       </c>
       <c r="B75" s="7">
-        <v>42113</v>
+        <v>42092</v>
       </c>
       <c r="C75" s="6" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="D75" s="6" t="s">
         <v>26</v>
       </c>
       <c r="E75" s="6" t="s">
-        <v>64</v>
+        <v>21</v>
       </c>
       <c r="F75" s="6" t="s">
         <v>16</v>
@@ -3535,24 +3541,24 @@
         <v>42156</v>
       </c>
       <c r="K75" s="6" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="76" spans="1:11" s="6" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="76" spans="1:11" s="6" customFormat="1" ht="96" x14ac:dyDescent="0.2">
       <c r="A76" s="6" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B76" s="7">
-        <v>42102</v>
-      </c>
-      <c r="C76" s="7" t="s">
-        <v>20</v>
+        <v>42113</v>
+      </c>
+      <c r="C76" s="6" t="s">
+        <v>12</v>
       </c>
       <c r="D76" s="6" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="E76" s="6" t="s">
-        <v>13</v>
+        <v>62</v>
       </c>
       <c r="F76" s="6" t="s">
         <v>16</v>
@@ -3563,53 +3569,120 @@
       <c r="H76" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="I76" s="7" t="s">
+      <c r="I76" s="6" t="s">
         <v>13</v>
       </c>
       <c r="J76" s="7">
         <v>42156</v>
       </c>
       <c r="K76" s="6" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="77" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.2">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="77" spans="1:11" s="6" customFormat="1" ht="24" x14ac:dyDescent="0.2">
       <c r="A77" s="6" t="s">
-        <v>68</v>
+        <v>166</v>
       </c>
       <c r="B77" s="7">
-        <v>42075</v>
+        <v>42102</v>
       </c>
       <c r="C77" s="7" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="D77" s="6" t="s">
         <v>13</v>
       </c>
       <c r="E77" s="6" t="s">
-        <v>35</v>
+        <v>13</v>
       </c>
       <c r="F77" s="6" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G77" s="6" t="s">
         <v>15</v>
       </c>
       <c r="H77" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="I77" s="6" t="s">
-        <v>22</v>
+        <v>13</v>
+      </c>
+      <c r="I77" s="7" t="s">
+        <v>13</v>
       </c>
       <c r="J77" s="7">
         <v>42156</v>
       </c>
       <c r="K77" s="6" t="s">
-        <v>69</v>
+        <v>167</v>
+      </c>
+    </row>
+    <row r="78" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A78" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="B78" s="7">
+        <v>42075</v>
+      </c>
+      <c r="C78" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D78" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E78" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="F78" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="G78" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="H78" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="I78" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="J78" s="7">
+        <v>42156</v>
+      </c>
+      <c r="K78" s="6" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="79" spans="1:11" s="6" customFormat="1" ht="36" x14ac:dyDescent="0.2">
+      <c r="A79" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="B79" s="7">
+        <v>42156</v>
+      </c>
+      <c r="C79" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D79" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="E79" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="F79" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="G79" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="H79" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="J79" s="7">
+        <v>42157</v>
+      </c>
+      <c r="K79" s="6" t="s">
+        <v>201</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:K44"/>
+  <autoFilter ref="A1:K45"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
@@ -3619,8 +3692,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:C14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3628,6 +3701,8 @@
     <col min="1" max="1" width="60.140625" customWidth="1"/>
     <col min="2" max="2" width="13.5703125" customWidth="1"/>
     <col min="3" max="3" width="77.42578125" customWidth="1"/>
+    <col min="9" max="9" width="9.140625" customWidth="1"/>
+    <col min="12" max="12" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">

</xml_diff>